<commit_message>
Update Plantilla Gestión del Proyecto.xlsx
</commit_message>
<xml_diff>
--- a/Diagrama Gant/Plantilla Gestión del Proyecto.xlsx
+++ b/Diagrama Gant/Plantilla Gestión del Proyecto.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose Damian\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{069D30F6-1E0F-4BD6-810D-E94A0EE418EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{377511E2-ED49-4F4A-9E47-30847E89E037}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,14 +26,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Informes '!$A$39:$G$43</definedName>
   </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -1802,30 +1794,8 @@
     <xf numFmtId="173" fontId="22" fillId="0" borderId="85" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="73" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1840,6 +1810,31 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1856,23 +1851,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="18" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="20" fillId="8" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="18" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="19" fillId="8" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="18" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1890,6 +1868,23 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="19" fillId="8" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="18" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="18" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="20" fillId="8" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="18" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="76" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1898,9 +1893,6 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="74" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="73" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2602,7 +2594,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1</c:v>
@@ -2611,7 +2603,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>2</c:v>
@@ -4360,8 +4352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1"/>
@@ -4386,16 +4378,16 @@
     <row r="1" spans="1:30" ht="21.75" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="140" t="s">
+      <c r="C1" s="130" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="141"/>
-      <c r="E1" s="141"/>
-      <c r="F1" s="141"/>
-      <c r="G1" s="141"/>
-      <c r="H1" s="141"/>
-      <c r="I1" s="141"/>
-      <c r="J1" s="142"/>
+      <c r="D1" s="131"/>
+      <c r="E1" s="131"/>
+      <c r="F1" s="131"/>
+      <c r="G1" s="131"/>
+      <c r="H1" s="131"/>
+      <c r="I1" s="131"/>
+      <c r="J1" s="132"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -4420,14 +4412,14 @@
     <row r="2" spans="1:30" ht="15.75">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="143"/>
-      <c r="D2" s="144"/>
-      <c r="E2" s="144"/>
-      <c r="F2" s="144"/>
-      <c r="G2" s="144"/>
-      <c r="H2" s="144"/>
-      <c r="I2" s="144"/>
-      <c r="J2" s="145"/>
+      <c r="C2" s="133"/>
+      <c r="D2" s="134"/>
+      <c r="E2" s="134"/>
+      <c r="F2" s="134"/>
+      <c r="G2" s="134"/>
+      <c r="H2" s="134"/>
+      <c r="I2" s="134"/>
+      <c r="J2" s="135"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -4558,15 +4550,15 @@
       <c r="B6" s="1"/>
       <c r="C6" s="6"/>
       <c r="D6" s="7"/>
-      <c r="E6" s="146" t="s">
+      <c r="E6" s="136" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="147"/>
-      <c r="G6" s="148"/>
-      <c r="H6" s="146" t="s">
+      <c r="F6" s="137"/>
+      <c r="G6" s="138"/>
+      <c r="H6" s="136" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="148"/>
+      <c r="I6" s="138"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -4672,10 +4664,10 @@
       <c r="B9" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="138" t="s">
+      <c r="C9" s="139" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="132"/>
+      <c r="D9" s="140"/>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
       <c r="G9" s="19"/>
@@ -4711,10 +4703,10 @@
       <c r="B10" s="16">
         <v>1</v>
       </c>
-      <c r="C10" s="129" t="s">
+      <c r="C10" s="141" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="130"/>
+      <c r="D10" s="142"/>
       <c r="E10" s="21">
         <v>43748</v>
       </c>
@@ -4758,10 +4750,10 @@
       <c r="B11" s="16">
         <v>2</v>
       </c>
-      <c r="C11" s="129" t="s">
+      <c r="C11" s="141" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="130"/>
+      <c r="D11" s="142"/>
       <c r="E11" s="24">
         <v>43775</v>
       </c>
@@ -4805,10 +4797,10 @@
       <c r="B12" s="16">
         <v>3</v>
       </c>
-      <c r="C12" s="139" t="s">
+      <c r="C12" s="143" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="137"/>
+      <c r="D12" s="144"/>
       <c r="E12" s="24">
         <v>43785</v>
       </c>
@@ -4855,10 +4847,10 @@
       <c r="B13" s="16">
         <v>4</v>
       </c>
-      <c r="C13" s="129" t="s">
+      <c r="C13" s="141" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="130"/>
+      <c r="D13" s="142"/>
       <c r="E13" s="24"/>
       <c r="F13" s="24"/>
       <c r="G13" s="22">
@@ -4901,10 +4893,10 @@
       <c r="B14" s="16">
         <v>5</v>
       </c>
-      <c r="C14" s="139" t="s">
+      <c r="C14" s="143" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="137"/>
+      <c r="D14" s="144"/>
       <c r="E14" s="24">
         <v>43971</v>
       </c>
@@ -4944,10 +4936,10 @@
     <row r="15" spans="1:30" ht="15.75">
       <c r="A15" s="1"/>
       <c r="B15" s="16"/>
-      <c r="C15" s="138" t="s">
+      <c r="C15" s="139" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="132"/>
+      <c r="D15" s="140"/>
       <c r="E15" s="24"/>
       <c r="F15" s="24"/>
       <c r="G15" s="22"/>
@@ -4983,10 +4975,10 @@
       <c r="B16" s="16">
         <v>6</v>
       </c>
-      <c r="C16" s="129" t="s">
+      <c r="C16" s="141" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="130"/>
+      <c r="D16" s="142"/>
       <c r="E16" s="24">
         <v>43961</v>
       </c>
@@ -5033,15 +5025,19 @@
       <c r="B17" s="16">
         <v>7</v>
       </c>
-      <c r="C17" s="129" t="s">
+      <c r="C17" s="141" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="130"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
+      <c r="D17" s="142"/>
+      <c r="E17" s="24">
+        <v>44053</v>
+      </c>
+      <c r="F17" s="24">
+        <v>44054</v>
+      </c>
       <c r="G17" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" s="19" t="s">
         <v>26</v>
@@ -5079,10 +5075,10 @@
       <c r="B18" s="16">
         <v>8</v>
       </c>
-      <c r="C18" s="129" t="s">
+      <c r="C18" s="141" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="130"/>
+      <c r="D18" s="142"/>
       <c r="E18" s="24">
         <v>44002</v>
       </c>
@@ -5126,10 +5122,10 @@
       <c r="B19" s="16">
         <v>9</v>
       </c>
-      <c r="C19" s="129" t="s">
+      <c r="C19" s="141" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="130"/>
+      <c r="D19" s="142"/>
       <c r="E19" s="24">
         <v>44004</v>
       </c>
@@ -5173,15 +5169,19 @@
       <c r="B20" s="16">
         <v>10</v>
       </c>
-      <c r="C20" s="135" t="s">
+      <c r="C20" s="148" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="132"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
+      <c r="D20" s="140"/>
+      <c r="E20" s="24">
+        <v>44056</v>
+      </c>
+      <c r="F20" s="24">
+        <v>44057</v>
+      </c>
       <c r="G20" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" s="19" t="s">
         <v>31</v>
@@ -5216,10 +5216,10 @@
       <c r="B21" s="16">
         <v>11</v>
       </c>
-      <c r="C21" s="135" t="s">
+      <c r="C21" s="148" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="132"/>
+      <c r="D21" s="140"/>
       <c r="E21" s="24">
         <v>43985</v>
       </c>
@@ -5263,10 +5263,10 @@
       <c r="B22" s="16">
         <v>12</v>
       </c>
-      <c r="C22" s="129" t="s">
+      <c r="C22" s="141" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="130"/>
+      <c r="D22" s="142"/>
       <c r="E22" s="24"/>
       <c r="F22" s="24"/>
       <c r="G22" s="22">
@@ -5304,10 +5304,10 @@
     <row r="23" spans="1:30" ht="15.75">
       <c r="A23" s="1"/>
       <c r="B23" s="16"/>
-      <c r="C23" s="136" t="s">
+      <c r="C23" s="149" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="137"/>
+      <c r="D23" s="144"/>
       <c r="E23" s="24"/>
       <c r="F23" s="24"/>
       <c r="G23" s="22"/>
@@ -5343,10 +5343,10 @@
       <c r="B24" s="16">
         <v>13</v>
       </c>
-      <c r="C24" s="129" t="s">
+      <c r="C24" s="141" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="130"/>
+      <c r="D24" s="142"/>
       <c r="E24" s="24"/>
       <c r="F24" s="24"/>
       <c r="G24" s="22">
@@ -5389,10 +5389,10 @@
       <c r="B25" s="16">
         <v>14</v>
       </c>
-      <c r="C25" s="129" t="s">
+      <c r="C25" s="141" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="130"/>
+      <c r="D25" s="142"/>
       <c r="E25" s="24"/>
       <c r="F25" s="24"/>
       <c r="G25" s="22">
@@ -5433,10 +5433,10 @@
     <row r="26" spans="1:30" ht="15.75">
       <c r="A26" s="1"/>
       <c r="B26" s="16"/>
-      <c r="C26" s="138" t="s">
+      <c r="C26" s="139" t="s">
         <v>40</v>
       </c>
-      <c r="D26" s="132"/>
+      <c r="D26" s="140"/>
       <c r="E26" s="24"/>
       <c r="F26" s="24"/>
       <c r="G26" s="22"/>
@@ -5472,10 +5472,10 @@
       <c r="B27" s="16">
         <v>15</v>
       </c>
-      <c r="C27" s="129" t="s">
+      <c r="C27" s="141" t="s">
         <v>41</v>
       </c>
-      <c r="D27" s="130"/>
+      <c r="D27" s="142"/>
       <c r="E27" s="24"/>
       <c r="F27" s="24"/>
       <c r="G27" s="22">
@@ -5518,10 +5518,10 @@
       <c r="B28" s="16">
         <v>16</v>
       </c>
-      <c r="C28" s="129" t="s">
+      <c r="C28" s="141" t="s">
         <v>43</v>
       </c>
-      <c r="D28" s="130"/>
+      <c r="D28" s="142"/>
       <c r="E28" s="24"/>
       <c r="F28" s="24"/>
       <c r="G28" s="22">
@@ -5562,8 +5562,8 @@
     <row r="29" spans="1:30" ht="15.75">
       <c r="A29" s="1"/>
       <c r="B29" s="26"/>
-      <c r="C29" s="131"/>
-      <c r="D29" s="132"/>
+      <c r="C29" s="145"/>
+      <c r="D29" s="140"/>
       <c r="E29" s="27"/>
       <c r="F29" s="27"/>
       <c r="G29" s="22"/>
@@ -5594,10 +5594,10 @@
     <row r="30" spans="1:30" ht="15.75">
       <c r="A30" s="1"/>
       <c r="B30" s="29"/>
-      <c r="C30" s="133" t="s">
+      <c r="C30" s="146" t="s">
         <v>45</v>
       </c>
-      <c r="D30" s="134"/>
+      <c r="D30" s="147"/>
       <c r="E30" s="30">
         <f>E11</f>
         <v>43775</v>
@@ -36676,21 +36676,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="C1:J2"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C27:D27"/>
     <mergeCell ref="C28:D28"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="C30:D30"/>
@@ -36701,6 +36686,21 @@
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C1:J2"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -36711,7 +36711,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F44B13A-C233-4769-922E-A0462F8E2503}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8" defaultRowHeight="15.75"/>
   <cols>
@@ -36729,8 +36729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:M32"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1"/>
@@ -36752,11 +36752,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="15.75">
-      <c r="B2" s="149" t="s">
+      <c r="B2" s="150" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="150"/>
-      <c r="D2" s="151"/>
+      <c r="C2" s="151"/>
+      <c r="D2" s="152"/>
     </row>
     <row r="3" spans="2:12" ht="5.25" customHeight="1"/>
     <row r="4" spans="2:12" ht="18.75" customHeight="1">
@@ -36769,15 +36769,15 @@
       <c r="D4" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="152" t="s">
+      <c r="F4" s="153" t="s">
         <v>50</v>
       </c>
-      <c r="G4" s="153"/>
-      <c r="H4" s="153"/>
-      <c r="I4" s="153"/>
-      <c r="J4" s="153"/>
-      <c r="K4" s="153"/>
-      <c r="L4" s="154"/>
+      <c r="G4" s="154"/>
+      <c r="H4" s="154"/>
+      <c r="I4" s="154"/>
+      <c r="J4" s="154"/>
+      <c r="K4" s="154"/>
+      <c r="L4" s="155"/>
     </row>
     <row r="5" spans="2:12" ht="15.75">
       <c r="B5" s="42" t="s">
@@ -36789,13 +36789,13 @@
       <c r="D5" s="44">
         <v>4000</v>
       </c>
-      <c r="F5" s="155"/>
-      <c r="G5" s="156"/>
-      <c r="H5" s="156"/>
-      <c r="I5" s="156"/>
-      <c r="J5" s="156"/>
-      <c r="K5" s="156"/>
-      <c r="L5" s="157"/>
+      <c r="F5" s="156"/>
+      <c r="G5" s="157"/>
+      <c r="H5" s="157"/>
+      <c r="I5" s="157"/>
+      <c r="J5" s="157"/>
+      <c r="K5" s="157"/>
+      <c r="L5" s="158"/>
     </row>
     <row r="6" spans="2:12" ht="15.75">
       <c r="B6" s="42" t="s">
@@ -36807,13 +36807,13 @@
       <c r="D6" s="44">
         <v>4000</v>
       </c>
-      <c r="F6" s="155"/>
-      <c r="G6" s="156"/>
-      <c r="H6" s="156"/>
-      <c r="I6" s="156"/>
-      <c r="J6" s="156"/>
-      <c r="K6" s="156"/>
-      <c r="L6" s="157"/>
+      <c r="F6" s="156"/>
+      <c r="G6" s="157"/>
+      <c r="H6" s="157"/>
+      <c r="I6" s="157"/>
+      <c r="J6" s="157"/>
+      <c r="K6" s="157"/>
+      <c r="L6" s="158"/>
     </row>
     <row r="7" spans="2:12" ht="15.75">
       <c r="B7" s="42" t="s">
@@ -36825,13 +36825,13 @@
       <c r="D7" s="44">
         <v>4000</v>
       </c>
-      <c r="F7" s="155"/>
-      <c r="G7" s="156"/>
-      <c r="H7" s="156"/>
-      <c r="I7" s="156"/>
-      <c r="J7" s="156"/>
-      <c r="K7" s="156"/>
-      <c r="L7" s="157"/>
+      <c r="F7" s="156"/>
+      <c r="G7" s="157"/>
+      <c r="H7" s="157"/>
+      <c r="I7" s="157"/>
+      <c r="J7" s="157"/>
+      <c r="K7" s="157"/>
+      <c r="L7" s="158"/>
     </row>
     <row r="8" spans="2:12" ht="15.75">
       <c r="B8" s="108" t="s">
@@ -36843,13 +36843,13 @@
       <c r="D8" s="107">
         <v>4000</v>
       </c>
-      <c r="F8" s="158"/>
-      <c r="G8" s="159"/>
-      <c r="H8" s="159"/>
-      <c r="I8" s="159"/>
-      <c r="J8" s="159"/>
-      <c r="K8" s="159"/>
-      <c r="L8" s="160"/>
+      <c r="F8" s="159"/>
+      <c r="G8" s="160"/>
+      <c r="H8" s="160"/>
+      <c r="I8" s="160"/>
+      <c r="J8" s="160"/>
+      <c r="K8" s="160"/>
+      <c r="L8" s="161"/>
     </row>
     <row r="9" spans="2:12" ht="9.75" customHeight="1"/>
     <row r="10" spans="2:12" ht="15.75">
@@ -37071,10 +37071,18 @@
         <f>Planificación!C20</f>
         <v>Diccionario de Datos</v>
       </c>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
+      <c r="C21" s="43">
+        <v>0.4</v>
+      </c>
+      <c r="D21" s="43">
+        <v>0.4</v>
+      </c>
+      <c r="E21" s="43">
+        <v>0.4</v>
+      </c>
+      <c r="F21" s="43">
+        <v>0.5</v>
+      </c>
       <c r="G21" s="49"/>
     </row>
     <row r="22" spans="2:13" ht="15.75">
@@ -37193,7 +37201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:O29"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -37211,19 +37219,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15">
-      <c r="L2" s="168" t="s">
+      <c r="L2" s="162" t="s">
         <v>52</v>
       </c>
-      <c r="M2" s="170">
+      <c r="M2" s="164">
         <f>M7</f>
         <v>573200</v>
       </c>
-      <c r="N2" s="154"/>
+      <c r="N2" s="155"/>
     </row>
     <row r="3" spans="2:15">
-      <c r="L3" s="169"/>
-      <c r="M3" s="158"/>
-      <c r="N3" s="160"/>
+      <c r="L3" s="163"/>
+      <c r="M3" s="159"/>
+      <c r="N3" s="161"/>
     </row>
     <row r="4" spans="2:15">
       <c r="C4" s="53"/>
@@ -37239,26 +37247,26 @@
     </row>
     <row r="5" spans="2:15" ht="15.75">
       <c r="B5" s="6"/>
-      <c r="C5" s="171" t="s">
+      <c r="C5" s="165" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="147"/>
-      <c r="E5" s="148"/>
-      <c r="F5" s="171" t="s">
+      <c r="D5" s="137"/>
+      <c r="E5" s="138"/>
+      <c r="F5" s="165" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="147"/>
-      <c r="H5" s="147"/>
-      <c r="I5" s="148"/>
-      <c r="J5" s="172" t="s">
+      <c r="G5" s="137"/>
+      <c r="H5" s="137"/>
+      <c r="I5" s="138"/>
+      <c r="J5" s="166" t="s">
         <v>55</v>
       </c>
-      <c r="K5" s="147"/>
-      <c r="L5" s="148"/>
-      <c r="M5" s="173" t="s">
+      <c r="K5" s="137"/>
+      <c r="L5" s="138"/>
+      <c r="M5" s="167" t="s">
         <v>56</v>
       </c>
-      <c r="N5" s="173" t="s">
+      <c r="N5" s="167" t="s">
         <v>57</v>
       </c>
       <c r="O5" s="55" t="s">
@@ -37299,8 +37307,8 @@
       <c r="L6" s="59" t="s">
         <v>61</v>
       </c>
-      <c r="M6" s="174"/>
-      <c r="N6" s="174"/>
+      <c r="M6" s="168"/>
+      <c r="N6" s="168"/>
       <c r="O6" s="61" t="s">
         <v>67</v>
       </c>
@@ -37337,21 +37345,21 @@
         <f>Planificación!C9</f>
         <v>FASE  DE ANALISIS</v>
       </c>
-      <c r="C8" s="161"/>
-      <c r="D8" s="162"/>
+      <c r="C8" s="171"/>
+      <c r="D8" s="172"/>
       <c r="E8" s="72">
         <f>SUM(E9:E12)</f>
         <v>360000</v>
       </c>
-      <c r="F8" s="163"/>
-      <c r="G8" s="150"/>
-      <c r="H8" s="151"/>
+      <c r="F8" s="173"/>
+      <c r="G8" s="151"/>
+      <c r="H8" s="152"/>
       <c r="I8" s="72">
         <f>SUM(I9:I12)</f>
         <v>43200</v>
       </c>
-      <c r="J8" s="164"/>
-      <c r="K8" s="165"/>
+      <c r="J8" s="174"/>
+      <c r="K8" s="175"/>
       <c r="L8" s="73">
         <f>SUM(L9:L12)</f>
         <v>15000</v>
@@ -37546,21 +37554,21 @@
         <f>Planificación!C15</f>
         <v>FASE DE DISEÑO</v>
       </c>
-      <c r="C13" s="161"/>
-      <c r="D13" s="162"/>
+      <c r="C13" s="171"/>
+      <c r="D13" s="172"/>
       <c r="E13" s="72">
         <f>SUM(E14:E20)</f>
         <v>155000</v>
       </c>
-      <c r="F13" s="166"/>
-      <c r="G13" s="150"/>
-      <c r="H13" s="151"/>
+      <c r="F13" s="169"/>
+      <c r="G13" s="151"/>
+      <c r="H13" s="152"/>
       <c r="I13" s="72">
         <f>SUM(I14:I20)</f>
         <v>0</v>
       </c>
-      <c r="J13" s="167"/>
-      <c r="K13" s="132"/>
+      <c r="J13" s="170"/>
+      <c r="K13" s="140"/>
       <c r="L13" s="72">
         <f>SUM(L14:L20)</f>
         <v>0</v>
@@ -37834,21 +37842,21 @@
         <f>Planificación!C23</f>
         <v>FASE DESARROLLO</v>
       </c>
-      <c r="C21" s="161"/>
-      <c r="D21" s="162"/>
+      <c r="C21" s="171"/>
+      <c r="D21" s="172"/>
       <c r="E21" s="72">
         <f>SUM(E22:E23)</f>
         <v>0</v>
       </c>
-      <c r="F21" s="166"/>
-      <c r="G21" s="150"/>
-      <c r="H21" s="151"/>
+      <c r="F21" s="169"/>
+      <c r="G21" s="151"/>
+      <c r="H21" s="152"/>
       <c r="I21" s="72">
         <f>SUM(I22:I23)</f>
         <v>0</v>
       </c>
-      <c r="J21" s="167"/>
-      <c r="K21" s="132"/>
+      <c r="J21" s="170"/>
+      <c r="K21" s="140"/>
       <c r="L21" s="72">
         <f>SUM(L22:L23)</f>
         <v>0</v>
@@ -37936,21 +37944,21 @@
         <f>Planificación!C26</f>
         <v>FASE DE PRUEBAS / INTEGRACIÓN</v>
       </c>
-      <c r="C24" s="161"/>
-      <c r="D24" s="162"/>
+      <c r="C24" s="171"/>
+      <c r="D24" s="172"/>
       <c r="E24" s="72">
         <f>SUM(E25:E26)</f>
         <v>0</v>
       </c>
-      <c r="F24" s="166"/>
-      <c r="G24" s="150"/>
-      <c r="H24" s="151"/>
+      <c r="F24" s="169"/>
+      <c r="G24" s="151"/>
+      <c r="H24" s="152"/>
       <c r="I24" s="72">
         <f>SUM(I25:I26)</f>
         <v>0</v>
       </c>
-      <c r="J24" s="167"/>
-      <c r="K24" s="132"/>
+      <c r="J24" s="170"/>
+      <c r="K24" s="140"/>
       <c r="L24" s="72">
         <f>SUM(L25:L26)</f>
         <v>0</v>
@@ -38106,6 +38114,18 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="C21:D21"/>
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="M2:N3"/>
     <mergeCell ref="C5:E5"/>
@@ -38113,18 +38133,6 @@
     <mergeCell ref="J5:L5"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="J13:K13"/>
   </mergeCells>
   <conditionalFormatting sqref="O28:O29">
     <cfRule type="colorScale" priority="1">
@@ -38159,7 +38167,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C9A7C72-5424-466F-A730-084D260AE7AC}">
   <dimension ref="A24:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B38" sqref="B38:G38"/>
     </sheetView>
   </sheetViews>
@@ -38249,17 +38257,17 @@
     <row r="37" spans="1:7" ht="16.5" thickBot="1"/>
     <row r="38" spans="1:7">
       <c r="A38" s="113"/>
-      <c r="B38" s="175" t="s">
+      <c r="B38" s="176" t="s">
         <v>51</v>
       </c>
-      <c r="C38" s="176"/>
-      <c r="D38" s="176"/>
-      <c r="E38" s="176"/>
-      <c r="F38" s="176"/>
-      <c r="G38" s="177"/>
+      <c r="C38" s="177"/>
+      <c r="D38" s="177"/>
+      <c r="E38" s="177"/>
+      <c r="F38" s="177"/>
+      <c r="G38" s="178"/>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="178" t="s">
+      <c r="A39" s="129" t="s">
         <v>47</v>
       </c>
       <c r="B39" s="124" t="s">

</xml_diff>